<commit_message>
mis à jour de quelque quelques entrées
</commit_message>
<xml_diff>
--- a/histoire urbaine digitale classification metiers.xlsx
+++ b/histoire urbaine digitale classification metiers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julien/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514AA7BA-D483-494A-AE51-13241607D608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E74D72-A7A4-4F4C-AC76-FC54E8BB5FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{F8C1197D-2F23-A149-83C2-4E70C5CFBE33}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{F8C1197D-2F23-A149-83C2-4E70C5CFBE33}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="109">
   <si>
     <t>rentiere</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>COUNT</t>
+  </si>
+  <si>
+    <t>service/rente</t>
   </si>
 </sst>
 </file>
@@ -743,12 +746,13 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1061,7 +1065,7 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1325,7 +1329,7 @@
         <v>80</v>
       </c>
       <c r="B72" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1490,8 +1494,8 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="315" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1581,7 +1585,7 @@
       </c>
       <c r="C7" s="3">
         <f>COUNTIF(data!B:B,A7)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
classé les métiers qui apparaissent au moins 3 fois
</commit_message>
<xml_diff>
--- a/histoire urbaine digitale classification metiers.xlsx
+++ b/histoire urbaine digitale classification metiers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julien/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien/Documents/GitHub/HUM-450-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E74D72-A7A4-4F4C-AC76-FC54E8BB5FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99843B68-A6AC-A54E-AC30-339DD742692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{F8C1197D-2F23-A149-83C2-4E70C5CFBE33}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
   <si>
     <t>rentiere</t>
   </si>
@@ -364,6 +364,108 @@
   </si>
   <si>
     <t>service/rente</t>
+  </si>
+  <si>
+    <t>musicien</t>
+  </si>
+  <si>
+    <t>orfevre</t>
+  </si>
+  <si>
+    <t>idt</t>
+  </si>
+  <si>
+    <t>henuisier</t>
+  </si>
+  <si>
+    <t>fileuse</t>
+  </si>
+  <si>
+    <t>bijoutier</t>
+  </si>
+  <si>
+    <t>fontenier</t>
+  </si>
+  <si>
+    <t>contrepointiere</t>
+  </si>
+  <si>
+    <t>rdinier</t>
+  </si>
+  <si>
+    <t>perruquier</t>
+  </si>
+  <si>
+    <t>charpents</t>
+  </si>
+  <si>
+    <t>charp</t>
+  </si>
+  <si>
+    <t>regent</t>
+  </si>
+  <si>
+    <t>maron</t>
+  </si>
+  <si>
+    <t>lessiveuse</t>
+  </si>
+  <si>
+    <t>architecte</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>relieur</t>
+  </si>
+  <si>
+    <t>peintre</t>
+  </si>
+  <si>
+    <t>canoeuvre</t>
+  </si>
+  <si>
+    <t>fraiteur</t>
+  </si>
+  <si>
+    <t>unier</t>
+  </si>
+  <si>
+    <t>taire</t>
+  </si>
+  <si>
+    <t>banquier</t>
+  </si>
+  <si>
+    <t>femme de menage</t>
+  </si>
+  <si>
+    <t>negociant</t>
+  </si>
+  <si>
+    <t>courtier</t>
+  </si>
+  <si>
+    <t>proprietaire|vigneron</t>
+  </si>
+  <si>
+    <t>gipseur</t>
+  </si>
+  <si>
+    <t>gipsier</t>
+  </si>
+  <si>
+    <t>chuprimeur</t>
+  </si>
+  <si>
+    <t>horloger</t>
+  </si>
+  <si>
+    <t>service/construction</t>
+  </si>
+  <si>
+    <t>artisanat/service</t>
   </si>
 </sst>
 </file>
@@ -744,10 +846,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78A07D2-6E35-C54E-9CBE-B63E15D42201}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="231" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,7 +1151,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1474,6 +1576,262 @@
       </c>
       <c r="B90" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>109</v>
+      </c>
+      <c r="B91" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>110</v>
+      </c>
+      <c r="B92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>112</v>
+      </c>
+      <c r="B94" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>113</v>
+      </c>
+      <c r="B95" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>115</v>
+      </c>
+      <c r="B97" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>116</v>
+      </c>
+      <c r="B98" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>117</v>
+      </c>
+      <c r="B99" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>121</v>
+      </c>
+      <c r="B103" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>122</v>
+      </c>
+      <c r="B104" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>123</v>
+      </c>
+      <c r="B105" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>124</v>
+      </c>
+      <c r="B106" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>125</v>
+      </c>
+      <c r="B107" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>126</v>
+      </c>
+      <c r="B108" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>127</v>
+      </c>
+      <c r="B109" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>128</v>
+      </c>
+      <c r="B110" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>129</v>
+      </c>
+      <c r="B111" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>130</v>
+      </c>
+      <c r="B112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>131</v>
+      </c>
+      <c r="B113" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>132</v>
+      </c>
+      <c r="B114" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>133</v>
+      </c>
+      <c r="B115" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>134</v>
+      </c>
+      <c r="B116" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>135</v>
+      </c>
+      <c r="B117" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>136</v>
+      </c>
+      <c r="B118" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>137</v>
+      </c>
+      <c r="B119" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>138</v>
+      </c>
+      <c r="B120" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>139</v>
+      </c>
+      <c r="B121" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>140</v>
+      </c>
+      <c r="B122" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1525,7 +1883,7 @@
       </c>
       <c r="C2" s="3">
         <f>COUNTIF(data!B:B,A2)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1537,7 +1895,7 @@
       </c>
       <c r="C3" s="3">
         <f>COUNTIF(data!B:B,A3)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1549,7 +1907,7 @@
       </c>
       <c r="C4" s="3">
         <f>COUNTIF(data!B:B,A4)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1561,7 +1919,7 @@
       </c>
       <c r="C5" s="3">
         <f>COUNTIF(data!B:B,A5)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1573,7 +1931,7 @@
       </c>
       <c r="C6" s="3">
         <f>COUNTIF(data!B:B,A6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1585,7 +1943,7 @@
       </c>
       <c r="C7" s="3">
         <f>COUNTIF(data!B:B,A7)</f>
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrigé un détail de la classification des métiers
</commit_message>
<xml_diff>
--- a/histoire urbaine digitale classification metiers.xlsx
+++ b/histoire urbaine digitale classification metiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien/Documents/GitHub/HUM-450-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99843B68-A6AC-A54E-AC30-339DD742692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4F0B99-EE29-934E-9D87-8B0970154070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{F8C1197D-2F23-A149-83C2-4E70C5CFBE33}"/>
   </bookViews>
@@ -848,8 +848,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="231" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>